<commit_message>
Hit a wall halfway through #3 on Chp 6. Next todo: vlookup median
</commit_message>
<xml_diff>
--- a/starwars_worked.xlsx
+++ b/starwars_worked.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcool\workspace\excel\data\starwars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBA48C9-83A0-46FD-B11F-6E76E6C2DD65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1020C0-58E2-4D18-801B-596487E5ABE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="starwars" sheetId="1" r:id="rId1"/>
@@ -1789,8 +1789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U93"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -8181,8 +8181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5FA28E1-BAA3-4B8B-A303-A05FEE6F2B32}">
   <dimension ref="A1:U87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updated and cleaned up visuals
</commit_message>
<xml_diff>
--- a/starwars_worked.xlsx
+++ b/starwars_worked.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcool\workspace\excel\data\starwars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1020C0-58E2-4D18-801B-596487E5ABE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEC5F3A-E295-4591-90A8-855BB9F7EEF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1789,8 +1789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="M61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -8181,8 +8181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5FA28E1-BAA3-4B8B-A303-A05FEE6F2B32}">
   <dimension ref="A1:U87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
hit a wall: Chp6#4. Skipping over for now
</commit_message>
<xml_diff>
--- a/starwars_worked.xlsx
+++ b/starwars_worked.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcool\workspace\excel\data\starwars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEC5F3A-E295-4591-90A8-855BB9F7EEF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCF385F-3965-40B2-91CF-1C8CD3B2B373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="starwars" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="291">
   <si>
     <t>name</t>
   </si>
@@ -918,6 +918,21 @@
   </si>
   <si>
     <t>midpoint</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>w/o functions</t>
+  </si>
+  <si>
+    <t>functions</t>
   </si>
 </sst>
 </file>
@@ -1071,7 +1086,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1263,6 +1278,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1424,7 +1445,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1432,6 +1453,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1477,7 +1499,18 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1789,7 +1822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M61" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="U17" sqref="U17"/>
     </sheetView>
   </sheetViews>
@@ -8179,16 +8212,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5FA28E1-BAA3-4B8B-A303-A05FEE6F2B32}">
-  <dimension ref="A1:U87"/>
+  <dimension ref="A1:U94"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="E89" sqref="E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.69921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="11.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -13522,6 +13557,11 @@
         <v>The Phantom Menace</v>
       </c>
     </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="C85" s="7" t="s">
+        <v>289</v>
+      </c>
+    </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C86" s="6" t="s">
         <v>283</v>
@@ -13539,9 +13579,71 @@
         <f>COUNT(D2:D82)/2</f>
         <v>40.5</v>
       </c>
+      <c r="G87">
+        <f>VLOOKUP(D87,C2:U82,2,TRUE)</f>
+        <v>180</v>
+      </c>
+      <c r="H87">
+        <f>VLOOKUP(39,C2:U82,2,TRUE)</f>
+        <v>180</v>
+      </c>
+      <c r="I87">
+        <f>VLOOKUP(43,C2:U82,2,TRUE)</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="C88" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="D88">
+        <f>VLOOKUP(D87,C2:U82,2,TRUE)</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="C89" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="91" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="C91" s="7" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="92" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="C92" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="D92">
+        <f>AVERAGE(D2:D82)</f>
+        <v>174.35802469135803</v>
+      </c>
+    </row>
+    <row r="93" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="C93" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="D93">
+        <f>MEDIAN(D2:D82)</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="94" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="C94" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="D94">
+        <f>_xlfn.MODE.SNGL(D2:D82)</f>
+        <v>183</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D2:D82">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Changed a vlookup for percentile. formatting
</commit_message>
<xml_diff>
--- a/starwars_worked.xlsx
+++ b/starwars_worked.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcool\workspace\excel\data\starwars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA939E98-14FB-4906-B681-34D5BB504A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8A5D7B-5A9B-448B-BE1F-366076C1492A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="starwars" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2126" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2127" uniqueCount="311">
   <si>
     <t>name</t>
   </si>
@@ -2283,7 +2283,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -8675,8 +8675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5FA28E1-BAA3-4B8B-A303-A05FEE6F2B32}">
   <dimension ref="A1:W96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="M89" sqref="M89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -8689,6 +8689,7 @@
     <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.09765625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="18" x14ac:dyDescent="0.35">
@@ -14757,6 +14758,9 @@
       <c r="M92" s="10" t="s">
         <v>300</v>
       </c>
+      <c r="O92" s="10" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="93" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A93" s="7" t="s">
@@ -14766,7 +14770,7 @@
         <v>295</v>
       </c>
       <c r="J93" s="9">
-        <f>ROUNDUP(COUNT(B4:B84)*0.9,0)</f>
+        <f>ROUND(COUNT(B4:B84)*0.9,0)</f>
         <v>73</v>
       </c>
       <c r="K93" s="9">
@@ -14779,6 +14783,10 @@
       <c r="N93" s="9">
         <f>ROUNDUP(COUNT(B4:B84)*0.25,0)</f>
         <v>21</v>
+      </c>
+      <c r="O93" s="9">
+        <f>VLOOKUP(N93,C4:W84,2)</f>
+        <v>167</v>
       </c>
     </row>
     <row r="94" spans="1:23" x14ac:dyDescent="0.3">

</xml_diff>